<commit_message>
lr: update tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Liberia/2024/lr_lf_tas_2410_2_fts.xlsx
+++ b/LF/TAS/Liberia/2024/lr_lf_tas_2410_2_fts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Liberia\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A50DFC-AC64-4AC9-BA32-EEE655F6CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004846DF-DBD6-4428-BD35-EFE3D938566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,15 +466,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>lr_lf_tas_2410_2_fts</t>
-  </si>
-  <si>
-    <t>lr_tas_fts_2410</t>
-  </si>
-  <si>
-    <t>(Sept 2024) 2. TAS2 FTS Form</t>
-  </si>
-  <si>
     <t>Select the community</t>
   </si>
   <si>
@@ -539,6 +530,15 @@
   </si>
   <si>
     <t>d_sleed_bed_net</t>
+  </si>
+  <si>
+    <t>lr_lf_tas_2410_2_fts_v2</t>
+  </si>
+  <si>
+    <t>(Sept 2024) 2. TAS2 FTS Form V2</t>
+  </si>
+  <si>
+    <t>lr_tas_fts_24102</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1214,7 +1214,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="28"/>
@@ -1236,7 +1236,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="28"/>
@@ -1276,7 +1276,7 @@
         <v>95</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>101</v>
@@ -1337,13 +1337,13 @@
     </row>
     <row r="10" spans="1:15" s="16" customFormat="1">
       <c r="A10" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D10" s="38"/>
       <c r="G10" s="38"/>
@@ -1357,14 +1357,14 @@
         <v>133</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J11" s="38" t="s">
         <v>16</v>
@@ -1375,13 +1375,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>16</v>
@@ -1395,7 +1395,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="29"/>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="H13" s="29"/>
       <c r="I13" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J13" s="28" t="s">
         <v>16</v>
@@ -1482,7 +1482,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="32"/>
       <c r="H16" s="29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="28" t="s">
@@ -1507,7 +1507,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="32"/>
       <c r="H17" s="29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="28" t="s">
@@ -1578,7 +1578,7 @@
       <c r="F20" s="28"/>
       <c r="G20" s="32"/>
       <c r="H20" s="29" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I20" s="28"/>
       <c r="J20" s="28" t="s">
@@ -1605,7 +1605,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="35"/>
       <c r="H21" s="29" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I21" s="33"/>
       <c r="J21" s="28" t="s">
@@ -1632,7 +1632,7 @@
       <c r="F22" s="33"/>
       <c r="G22" s="35"/>
       <c r="H22" s="29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I22" s="33"/>
       <c r="J22" s="28" t="s">
@@ -1659,7 +1659,7 @@
       <c r="F23" s="33"/>
       <c r="G23" s="35"/>
       <c r="H23" s="29" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I23" s="33"/>
       <c r="J23" s="28" t="s">
@@ -1721,7 +1721,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C27" s="36" t="s">
         <v>109</v>
@@ -1842,7 +1842,7 @@
         <v>100</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>126</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="30" spans="1:3" s="26" customFormat="1">
       <c r="A30" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>67</v>
@@ -2244,13 +2244,13 @@
     </row>
     <row r="31" spans="1:3" s="26" customFormat="1">
       <c r="A31" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3515,10 +3515,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
lr: tas update forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Liberia/2024/lr_lf_tas_2410_2_fts.xlsx
+++ b/LF/TAS/Liberia/2024/lr_lf_tas_2410_2_fts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Liberia\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004846DF-DBD6-4428-BD35-EFE3D938566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4721D0E-AD69-4D4C-BDAB-24A2C8EABFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="169">
   <si>
     <t>type</t>
   </si>
@@ -532,13 +532,19 @@
     <t>d_sleed_bed_net</t>
   </si>
   <si>
-    <t>lr_lf_tas_2410_2_fts_v2</t>
-  </si>
-  <si>
-    <t>(Sept 2024) 2. TAS2 FTS Form V2</t>
-  </si>
-  <si>
-    <t>lr_tas_fts_24102</t>
+    <t>(Sept 2024) 2. TAS2 FTS Form V3</t>
+  </si>
+  <si>
+    <t>lr_lf_tas_2410_2_fts_v3</t>
+  </si>
+  <si>
+    <t>lr_tas_fts_24103</t>
+  </si>
+  <si>
+    <t>Select the District</t>
+  </si>
+  <si>
+    <t>d_district</t>
   </si>
 </sst>
 </file>
@@ -1088,13 +1094,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1210,33 +1216,32 @@
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28" t="s">
+      <c r="B4" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
     </row>
     <row r="5" spans="1:15" s="16" customFormat="1">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="30"/>
       <c r="E5" s="28"/>
@@ -1251,75 +1256,76 @@
       <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:15" s="16" customFormat="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+    </row>
+    <row r="7" spans="1:15" s="16" customFormat="1">
+      <c r="A7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" s="16" customFormat="1">
-      <c r="A7" s="17" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" s="16" customFormat="1">
+      <c r="A8" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B8" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C8" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="22"/>
-    </row>
-    <row r="8" spans="1:15" s="16" customFormat="1">
-      <c r="A8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:15" s="16" customFormat="1">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
@@ -1328,7 +1334,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="11"/>
       <c r="I9" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
@@ -1336,128 +1342,124 @@
       <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:15" s="16" customFormat="1">
-      <c r="A10" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="29"/>
-      <c r="J10" s="38" t="s">
-        <v>16</v>
-      </c>
+      <c r="A10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:15" s="16" customFormat="1">
       <c r="A11" s="16" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="38"/>
-      <c r="H11" s="38" t="s">
-        <v>150</v>
-      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="29"/>
       <c r="J11" s="38" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="16" customFormat="1">
       <c r="A12" s="16" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>147</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D12" s="38"/>
       <c r="H12" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="16" customFormat="1" ht="31.5">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:15" s="16" customFormat="1">
+      <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="J13" s="28" t="s">
+      <c r="B13" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="16" customFormat="1">
+    </row>
+    <row r="14" spans="1:15" s="16" customFormat="1" ht="31.5">
       <c r="A14" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="D14" s="30"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="I14" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="J14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="28"/>
-    </row>
-    <row r="15" spans="1:15" s="16" customFormat="1" ht="31.5">
+      <c r="N14" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="16" customFormat="1">
       <c r="A15" s="28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>26</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D15" s="30"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="32"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
       <c r="J15" s="28" t="s">
@@ -1467,23 +1469,23 @@
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
     </row>
-    <row r="16" spans="1:15" s="16" customFormat="1">
+    <row r="16" spans="1:15" s="16" customFormat="1" ht="31.5">
       <c r="A16" s="28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="30"/>
+        <v>25</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="32"/>
-      <c r="H16" s="29" t="s">
-        <v>156</v>
-      </c>
+      <c r="H16" s="29"/>
       <c r="I16" s="29"/>
       <c r="J16" s="28" t="s">
         <v>16</v>
@@ -1494,10 +1496,10 @@
     </row>
     <row r="17" spans="1:13" s="16" customFormat="1">
       <c r="A17" s="28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>29</v>
@@ -1507,7 +1509,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="32"/>
       <c r="H17" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="28" t="s">
@@ -1519,20 +1521,22 @@
     </row>
     <row r="18" spans="1:13" s="16" customFormat="1">
       <c r="A18" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="D18" s="30"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="32"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="28" t="s">
-        <v>34</v>
-      </c>
+      <c r="H18" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" s="29"/>
       <c r="J18" s="28" t="s">
         <v>16</v>
       </c>
@@ -1540,99 +1544,95 @@
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
     </row>
-    <row r="19" spans="1:13" s="16" customFormat="1" ht="63">
+    <row r="19" spans="1:13" s="16" customFormat="1">
       <c r="A19" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="35"/>
+        <v>32</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="32"/>
-      <c r="H19" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1">
+    <row r="20" spans="1:13" s="16" customFormat="1" ht="63">
       <c r="A20" s="28" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
       <c r="G20" s="32"/>
       <c r="H20" s="29" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="I20" s="28"/>
-      <c r="J20" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="J20" s="28"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" s="16" customFormat="1">
       <c r="A21" s="28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="35"/>
+        <v>40</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="I21" s="33"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
       <c r="G22" s="35"/>
       <c r="H22" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I22" s="33"/>
       <c r="J22" s="28" t="s">
@@ -1644,22 +1644,22 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E23" s="33"/>
       <c r="F23" s="33"/>
       <c r="G23" s="35"/>
       <c r="H23" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I23" s="33"/>
       <c r="J23" s="28" t="s">
@@ -1671,91 +1671,100 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
+        <v>46</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
       <c r="G24" s="35"/>
       <c r="H24" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="33"/>
+        <v>160</v>
+      </c>
+      <c r="I24" s="33"/>
+      <c r="J24" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="K24" s="33"/>
       <c r="L24" s="33"/>
       <c r="M24" s="33"/>
     </row>
-    <row r="25" spans="1:13" ht="56.25" customHeight="1">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+    </row>
+    <row r="26" spans="1:13" ht="56.25" customHeight="1">
+      <c r="A26" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="38"/>
-      <c r="I25" s="27" t="s">
+      <c r="H26" s="38"/>
+      <c r="I26" s="27" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="38"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>162</v>
+        <v>51</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="H27" s="38"/>
-      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="16" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>108</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="H28" s="38"/>
       <c r="I28" s="27"/>
-      <c r="J28" s="26" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="16" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="H29" s="29" t="s">
         <v>108</v>
@@ -1767,13 +1776,13 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>108</v>
@@ -1785,13 +1794,13 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="16" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="H31" s="29" t="s">
         <v>108</v>
@@ -1803,16 +1812,16 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="16" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I32" s="27"/>
       <c r="J32" s="26" t="s">
@@ -1821,16 +1830,16 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="16" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I33" s="27"/>
       <c r="J33" s="26" t="s">
@@ -1842,10 +1851,10 @@
         <v>100</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H34" s="29" t="s">
         <v>108</v>
@@ -1857,45 +1866,63 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="I35" s="27"/>
+      <c r="J35" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B36" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C36" s="36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:13">
+      <c r="A37" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>56</v>
-      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B39" s="26" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3488,7 +3515,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3515,10 +3542,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>165</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>164</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>92</v>

</xml_diff>